<commit_message>
Full Data table Master
</commit_message>
<xml_diff>
--- a/z_db/Data/Guru/guru.xlsx
+++ b/z_db/Data/Guru/guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\z_db\Data\Guru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FBD873-695F-4065-929A-E5BC6A54343B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5751B21-4C22-4500-85C1-60795AC19350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB8EC23C-913C-423A-A975-EF6DBF0E2D76}"/>
   </bookViews>
@@ -1354,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EC24D4-2F95-4EB9-81CE-F112F4F100E1}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>